<commit_message>
Updated BOM and Readme for CPC1018 part
JLCPCB has now started stocking the CPC1018 part regularly, so it's no longer a part that needs to be special ordered.  I've updated the BOM and Readme for the 125B and the 1590B-SMD projects to accurately reflect that.  This is good!
</commit_message>
<xml_diff>
--- a/Hardware/GuitarPedal125b/pcb/BOM_JLCSMT_DaisySeedGuitarPedal125b.xlsx
+++ b/Hardware/GuitarPedal125b/pcb/BOM_JLCSMT_DaisySeedGuitarPedal125b.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshep/Dev/DaisySeedProjects/GuitarPedal125b/pcb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshep/Dev/DaisySeedProjects/Hardware/GuitarPedal125b/pcb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ECD584-DFAB-8E41-9007-B3A435A27898}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D2CB24-B078-2745-9592-AE8AF61A12F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68540" yWindow="3100" windowWidth="28800" windowHeight="21660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="760" windowWidth="28800" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,7 +345,7 @@
     <t>CPC1018N</t>
   </si>
   <si>
-    <t>C1558973</t>
+    <t>C133069</t>
   </si>
 </sst>
 </file>
@@ -871,7 +871,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>

</xml_diff>